<commit_message>
Ajout email users + modification PDF
</commit_message>
<xml_diff>
--- a/public/dependencies/includes/Fiche info projet.xlsx
+++ b/public/dependencies/includes/Fiche info projet.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\dev-requests\public\dependencies\includes\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{0C7746AF-5078-4855-A84A-3CAA81A41512}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12075"/>
+    <workbookView xWindow="120" yWindow="150" windowWidth="24920" windowHeight="12080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -14,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="43">
   <si>
     <t>DevReq</t>
   </si>
@@ -132,12 +138,24 @@
   </si>
   <si>
     <t>5 - REX</t>
+  </si>
+  <si>
+    <t>Type de données collectées et/ou utilisées</t>
+  </si>
+  <si>
+    <t>Finalité de la collecte et/ou de l'utilisation de ces données</t>
+  </si>
+  <si>
+    <t>Processus lié</t>
+  </si>
+  <si>
+    <t>Impact</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="8">
     <numFmt numFmtId="8" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
@@ -664,7 +682,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -676,23 +694,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -703,108 +731,116 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="78">
-    <cellStyle name="%" xfId="1"/>
-    <cellStyle name="% 2" xfId="2"/>
-    <cellStyle name="% 2 2" xfId="3"/>
-    <cellStyle name="20% - Accent1" xfId="4"/>
-    <cellStyle name="20% - Accent2" xfId="5"/>
-    <cellStyle name="20% - Accent3" xfId="6"/>
-    <cellStyle name="20% - Accent4" xfId="7"/>
-    <cellStyle name="20% - Accent5" xfId="8"/>
-    <cellStyle name="20% - Accent6" xfId="9"/>
-    <cellStyle name="40% - Accent1" xfId="10"/>
-    <cellStyle name="40% - Accent2" xfId="11"/>
-    <cellStyle name="40% - Accent3" xfId="12"/>
-    <cellStyle name="40% - Accent4" xfId="13"/>
-    <cellStyle name="40% - Accent5" xfId="14"/>
-    <cellStyle name="40% - Accent6" xfId="15"/>
-    <cellStyle name="60% - Accent1" xfId="16"/>
-    <cellStyle name="60% - Accent2" xfId="17"/>
-    <cellStyle name="60% - Accent3" xfId="18"/>
-    <cellStyle name="60% - Accent4" xfId="19"/>
-    <cellStyle name="60% - Accent5" xfId="20"/>
-    <cellStyle name="60% - Accent6" xfId="21"/>
-    <cellStyle name="Bad" xfId="22"/>
-    <cellStyle name="Calculation" xfId="23"/>
-    <cellStyle name="Calculation 2" xfId="24"/>
-    <cellStyle name="Calculation 2 2" xfId="25"/>
-    <cellStyle name="Calculation 3" xfId="26"/>
-    <cellStyle name="Check Cell" xfId="27"/>
-    <cellStyle name="Euro" xfId="28"/>
-    <cellStyle name="Euro 2" xfId="29"/>
-    <cellStyle name="Euro 2 2" xfId="30"/>
-    <cellStyle name="Explanatory Text" xfId="31"/>
-    <cellStyle name="Good" xfId="32"/>
-    <cellStyle name="Heading 1" xfId="33"/>
-    <cellStyle name="Heading 2" xfId="34"/>
-    <cellStyle name="Heading 3" xfId="35"/>
-    <cellStyle name="Heading 4" xfId="36"/>
-    <cellStyle name="Input" xfId="37"/>
-    <cellStyle name="Input 2" xfId="38"/>
-    <cellStyle name="Input 2 2" xfId="39"/>
-    <cellStyle name="Input 3" xfId="40"/>
-    <cellStyle name="Lien hypertexte 2" xfId="41"/>
-    <cellStyle name="Linked Cell" xfId="42"/>
-    <cellStyle name="Milliers 2" xfId="43"/>
-    <cellStyle name="Milliers 3" xfId="44"/>
-    <cellStyle name="Milliers 3 2" xfId="45"/>
-    <cellStyle name="Milliers 3 3" xfId="46"/>
-    <cellStyle name="Monétaire 2" xfId="47"/>
-    <cellStyle name="Monétaire 2 2" xfId="48"/>
-    <cellStyle name="Monétaire 2 3" xfId="49"/>
-    <cellStyle name="Neutral" xfId="50"/>
+    <cellStyle name="%" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="% 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="% 2 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="20% - Accent1" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="20% - Accent2" xfId="5" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="20% - Accent3" xfId="6" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="20% - Accent4" xfId="7" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="20% - Accent5" xfId="8" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="20% - Accent6" xfId="9" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="40% - Accent1" xfId="10" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="40% - Accent2" xfId="11" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
+    <cellStyle name="40% - Accent3" xfId="12" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
+    <cellStyle name="40% - Accent4" xfId="13" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
+    <cellStyle name="40% - Accent5" xfId="14" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
+    <cellStyle name="40% - Accent6" xfId="15" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
+    <cellStyle name="60% - Accent1" xfId="16" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
+    <cellStyle name="60% - Accent2" xfId="17" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
+    <cellStyle name="60% - Accent3" xfId="18" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
+    <cellStyle name="60% - Accent4" xfId="19" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
+    <cellStyle name="60% - Accent5" xfId="20" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
+    <cellStyle name="60% - Accent6" xfId="21" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
+    <cellStyle name="Bad" xfId="22" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
+    <cellStyle name="Calculation" xfId="23" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
+    <cellStyle name="Calculation 2" xfId="24" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
+    <cellStyle name="Calculation 2 2" xfId="25" xr:uid="{00000000-0005-0000-0000-000018000000}"/>
+    <cellStyle name="Calculation 3" xfId="26" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
+    <cellStyle name="Check Cell" xfId="27" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
+    <cellStyle name="Euro" xfId="28" xr:uid="{00000000-0005-0000-0000-00001B000000}"/>
+    <cellStyle name="Euro 2" xfId="29" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
+    <cellStyle name="Euro 2 2" xfId="30" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
+    <cellStyle name="Explanatory Text" xfId="31" xr:uid="{00000000-0005-0000-0000-00001E000000}"/>
+    <cellStyle name="Good" xfId="32" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
+    <cellStyle name="Heading 1" xfId="33" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
+    <cellStyle name="Heading 2" xfId="34" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
+    <cellStyle name="Heading 3" xfId="35" xr:uid="{00000000-0005-0000-0000-000022000000}"/>
+    <cellStyle name="Heading 4" xfId="36" xr:uid="{00000000-0005-0000-0000-000023000000}"/>
+    <cellStyle name="Input" xfId="37" xr:uid="{00000000-0005-0000-0000-000024000000}"/>
+    <cellStyle name="Input 2" xfId="38" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
+    <cellStyle name="Input 2 2" xfId="39" xr:uid="{00000000-0005-0000-0000-000026000000}"/>
+    <cellStyle name="Input 3" xfId="40" xr:uid="{00000000-0005-0000-0000-000027000000}"/>
+    <cellStyle name="Lien hypertexte 2" xfId="41" xr:uid="{00000000-0005-0000-0000-000028000000}"/>
+    <cellStyle name="Linked Cell" xfId="42" xr:uid="{00000000-0005-0000-0000-000029000000}"/>
+    <cellStyle name="Milliers 2" xfId="43" xr:uid="{00000000-0005-0000-0000-00002A000000}"/>
+    <cellStyle name="Milliers 3" xfId="44" xr:uid="{00000000-0005-0000-0000-00002B000000}"/>
+    <cellStyle name="Milliers 3 2" xfId="45" xr:uid="{00000000-0005-0000-0000-00002C000000}"/>
+    <cellStyle name="Milliers 3 3" xfId="46" xr:uid="{00000000-0005-0000-0000-00002D000000}"/>
+    <cellStyle name="Monétaire 2" xfId="47" xr:uid="{00000000-0005-0000-0000-00002E000000}"/>
+    <cellStyle name="Monétaire 2 2" xfId="48" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
+    <cellStyle name="Monétaire 2 3" xfId="49" xr:uid="{00000000-0005-0000-0000-000030000000}"/>
+    <cellStyle name="Neutral" xfId="50" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="51"/>
-    <cellStyle name="Normal 2 2" xfId="52"/>
-    <cellStyle name="Normal 3" xfId="53"/>
-    <cellStyle name="Normal 3 2" xfId="54"/>
-    <cellStyle name="Normal 4" xfId="55"/>
-    <cellStyle name="Normal 5" xfId="56"/>
-    <cellStyle name="Note" xfId="57"/>
-    <cellStyle name="Note 2" xfId="58"/>
-    <cellStyle name="Note 2 2" xfId="59"/>
-    <cellStyle name="Note 2 2 2" xfId="60"/>
-    <cellStyle name="Note 2 3" xfId="61"/>
-    <cellStyle name="Note 3" xfId="62"/>
-    <cellStyle name="Note 3 2" xfId="63"/>
-    <cellStyle name="Note 3 2 2" xfId="64"/>
-    <cellStyle name="Note 3 3" xfId="65"/>
-    <cellStyle name="Note 4" xfId="66"/>
-    <cellStyle name="Note 4 2" xfId="67"/>
-    <cellStyle name="Note 5" xfId="68"/>
-    <cellStyle name="Output" xfId="69"/>
-    <cellStyle name="Output 2" xfId="70"/>
-    <cellStyle name="Output 2 2" xfId="71"/>
-    <cellStyle name="Output 3" xfId="72"/>
-    <cellStyle name="Pourcentage 2" xfId="73"/>
-    <cellStyle name="Pourcentage 3" xfId="74"/>
-    <cellStyle name="Title" xfId="75"/>
-    <cellStyle name="Titre 1" xfId="76"/>
-    <cellStyle name="Warning Text" xfId="77"/>
+    <cellStyle name="Normal 2" xfId="51" xr:uid="{00000000-0005-0000-0000-000033000000}"/>
+    <cellStyle name="Normal 2 2" xfId="52" xr:uid="{00000000-0005-0000-0000-000034000000}"/>
+    <cellStyle name="Normal 3" xfId="53" xr:uid="{00000000-0005-0000-0000-000035000000}"/>
+    <cellStyle name="Normal 3 2" xfId="54" xr:uid="{00000000-0005-0000-0000-000036000000}"/>
+    <cellStyle name="Normal 4" xfId="55" xr:uid="{00000000-0005-0000-0000-000037000000}"/>
+    <cellStyle name="Normal 5" xfId="56" xr:uid="{00000000-0005-0000-0000-000038000000}"/>
+    <cellStyle name="Note" xfId="57" xr:uid="{00000000-0005-0000-0000-000039000000}"/>
+    <cellStyle name="Note 2" xfId="58" xr:uid="{00000000-0005-0000-0000-00003A000000}"/>
+    <cellStyle name="Note 2 2" xfId="59" xr:uid="{00000000-0005-0000-0000-00003B000000}"/>
+    <cellStyle name="Note 2 2 2" xfId="60" xr:uid="{00000000-0005-0000-0000-00003C000000}"/>
+    <cellStyle name="Note 2 3" xfId="61" xr:uid="{00000000-0005-0000-0000-00003D000000}"/>
+    <cellStyle name="Note 3" xfId="62" xr:uid="{00000000-0005-0000-0000-00003E000000}"/>
+    <cellStyle name="Note 3 2" xfId="63" xr:uid="{00000000-0005-0000-0000-00003F000000}"/>
+    <cellStyle name="Note 3 2 2" xfId="64" xr:uid="{00000000-0005-0000-0000-000040000000}"/>
+    <cellStyle name="Note 3 3" xfId="65" xr:uid="{00000000-0005-0000-0000-000041000000}"/>
+    <cellStyle name="Note 4" xfId="66" xr:uid="{00000000-0005-0000-0000-000042000000}"/>
+    <cellStyle name="Note 4 2" xfId="67" xr:uid="{00000000-0005-0000-0000-000043000000}"/>
+    <cellStyle name="Note 5" xfId="68" xr:uid="{00000000-0005-0000-0000-000044000000}"/>
+    <cellStyle name="Output" xfId="69" xr:uid="{00000000-0005-0000-0000-000045000000}"/>
+    <cellStyle name="Output 2" xfId="70" xr:uid="{00000000-0005-0000-0000-000046000000}"/>
+    <cellStyle name="Output 2 2" xfId="71" xr:uid="{00000000-0005-0000-0000-000047000000}"/>
+    <cellStyle name="Output 3" xfId="72" xr:uid="{00000000-0005-0000-0000-000048000000}"/>
+    <cellStyle name="Pourcentage 2" xfId="73" xr:uid="{00000000-0005-0000-0000-000049000000}"/>
+    <cellStyle name="Pourcentage 3" xfId="74" xr:uid="{00000000-0005-0000-0000-00004A000000}"/>
+    <cellStyle name="Title" xfId="75" xr:uid="{00000000-0005-0000-0000-00004B000000}"/>
+    <cellStyle name="Titre 1" xfId="76" xr:uid="{00000000-0005-0000-0000-00004C000000}"/>
+    <cellStyle name="Warning Text" xfId="77" xr:uid="{00000000-0005-0000-0000-00004D000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -827,7 +863,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Image 2"/>
+        <xdr:cNvPr id="3" name="Image 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -902,7 +944,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -935,9 +977,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -970,6 +1029,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1145,32 +1221,53 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L54"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:X54"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScale="55" zoomScaleNormal="70" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="55" workbookViewId="0">
+      <selection activeCell="I39" sqref="I39:J39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.42578125" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" customWidth="1"/>
-    <col min="3" max="3" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="7" width="5.7109375" customWidth="1"/>
-    <col min="9" max="11" width="5.7109375" style="11" customWidth="1"/>
-    <col min="12" max="12" width="5.5703125" customWidth="1"/>
+    <col min="1" max="1" width="8.453125" customWidth="1"/>
+    <col min="2" max="2" width="11.1796875" customWidth="1"/>
+    <col min="3" max="3" width="21.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="5.7265625" customWidth="1"/>
+    <col min="9" max="11" width="5.7265625" style="10" customWidth="1"/>
+    <col min="12" max="12" width="5.54296875" customWidth="1"/>
+    <col min="13" max="13" width="8.453125" style="10" customWidth="1"/>
+    <col min="14" max="14" width="11.1796875" style="10" customWidth="1"/>
+    <col min="15" max="15" width="21.54296875" style="10" bestFit="1" customWidth="1"/>
+    <col min="16" max="19" width="5.7265625" style="10" customWidth="1"/>
+    <col min="20" max="20" width="10.90625" style="10"/>
+    <col min="21" max="23" width="5.7265625" style="10" customWidth="1"/>
+    <col min="24" max="24" width="5.54296875" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="28" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3"/>
+      <c r="V1" s="3"/>
+      <c r="W1" s="3"/>
+      <c r="X1" s="3"/>
+    </row>
+    <row r="2" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
-      <c r="B2" s="16"/>
+      <c r="B2" s="28"/>
       <c r="D2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1183,65 +1280,177 @@
       <c r="K2" s="6"/>
       <c r="L2" s="6"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
-      <c r="B4" s="6"/>
+    <row r="3" spans="1:24" ht="39" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="N3" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="O3" s="21"/>
+      <c r="P3" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q3" s="25"/>
+      <c r="R3" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="S3" s="25"/>
+      <c r="T3" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="U3" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="V3" s="21"/>
+      <c r="W3" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="X3" s="26"/>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A4" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="10"/>
       <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4" s="10"/>
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
       <c r="K4" s="6"/>
       <c r="L4" s="6"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
+      <c r="N4" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="O4" s="22"/>
+      <c r="P4" s="27"/>
+      <c r="Q4" s="27"/>
+      <c r="R4" s="23"/>
+      <c r="S4" s="23"/>
+      <c r="T4" s="9"/>
+      <c r="U4" s="23"/>
+      <c r="V4" s="23"/>
+      <c r="W4" s="23"/>
+      <c r="X4" s="23"/>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A5" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="10"/>
       <c r="C5" s="6"/>
-      <c r="G5" t="s">
-        <v>2</v>
-      </c>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="H5" s="10"/>
       <c r="I5" s="6"/>
       <c r="J5" s="6"/>
       <c r="K5" s="6"/>
       <c r="L5" s="6"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="6"/>
-      <c r="G6" t="s">
-        <v>3</v>
-      </c>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="6"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="N5" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="O5" s="22"/>
+      <c r="P5" s="23"/>
+      <c r="Q5" s="23"/>
+      <c r="R5" s="23"/>
+      <c r="S5" s="23"/>
+      <c r="T5" s="9"/>
+      <c r="U5" s="23"/>
+      <c r="V5" s="23"/>
+      <c r="W5" s="23"/>
+      <c r="X5" s="23"/>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A6" s="10"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="L6" s="10"/>
+      <c r="N6" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="O6" s="22"/>
+      <c r="P6" s="23"/>
+      <c r="Q6" s="23"/>
+      <c r="R6" s="23"/>
+      <c r="S6" s="23"/>
+      <c r="T6" s="9"/>
+      <c r="U6" s="23"/>
+      <c r="V6" s="23"/>
+      <c r="W6" s="23"/>
+      <c r="X6" s="23"/>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A7" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-    </row>
-    <row r="9" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="B9" s="6"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="N7" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="O7" s="22"/>
+      <c r="P7" s="23"/>
+      <c r="Q7" s="23"/>
+      <c r="R7" s="23"/>
+      <c r="S7" s="23"/>
+      <c r="T7" s="9"/>
+      <c r="U7" s="23"/>
+      <c r="V7" s="23"/>
+      <c r="W7" s="23"/>
+      <c r="X7" s="23"/>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A8" s="5"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="N8" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="O8" s="22"/>
+      <c r="P8" s="23"/>
+      <c r="Q8" s="23"/>
+      <c r="R8" s="23"/>
+      <c r="S8" s="23"/>
+      <c r="T8" s="9"/>
+      <c r="U8" s="23"/>
+      <c r="V8" s="23"/>
+      <c r="W8" s="23"/>
+      <c r="X8" s="23"/>
+    </row>
+    <row r="9" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="10" t="s">
+        <v>6</v>
+      </c>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
@@ -1252,11 +1461,23 @@
       <c r="J9" s="6"/>
       <c r="K9" s="6"/>
       <c r="L9" s="6"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>6</v>
-      </c>
+      <c r="N9" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="O9" s="22"/>
+      <c r="P9" s="23"/>
+      <c r="Q9" s="23"/>
+      <c r="R9" s="23"/>
+      <c r="S9" s="23"/>
+      <c r="T9" s="9"/>
+      <c r="U9" s="23"/>
+      <c r="V9" s="23"/>
+      <c r="W9" s="23"/>
+      <c r="X9" s="23"/>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A10" s="10"/>
+      <c r="B10" s="10"/>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
@@ -1267,8 +1488,18 @@
       <c r="J10" s="6"/>
       <c r="K10" s="6"/>
       <c r="L10" s="6"/>
-    </row>
-    <row r="11" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="O10" s="14"/>
+      <c r="P10" s="15"/>
+      <c r="Q10" s="15"/>
+      <c r="R10" s="15"/>
+      <c r="S10" s="15"/>
+      <c r="T10" s="6"/>
+      <c r="U10" s="15"/>
+      <c r="V10" s="15"/>
+      <c r="W10" s="15"/>
+      <c r="X10" s="15"/>
+    </row>
+    <row r="11" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
@@ -1280,7 +1511,9 @@
       <c r="K11" s="6"/>
       <c r="L11" s="6"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A12" s="10"/>
+      <c r="B12" s="10"/>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
@@ -1291,8 +1524,22 @@
       <c r="J12" s="6"/>
       <c r="K12" s="6"/>
       <c r="L12" s="6"/>
-    </row>
-    <row r="13" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M12" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
+      <c r="P12" s="3"/>
+      <c r="Q12" s="3"/>
+      <c r="R12" s="3"/>
+      <c r="S12" s="3"/>
+      <c r="T12" s="3"/>
+      <c r="U12" s="3"/>
+      <c r="V12" s="3"/>
+      <c r="W12" s="3"/>
+      <c r="X12" s="3"/>
+    </row>
+    <row r="13" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
@@ -1303,11 +1550,22 @@
       <c r="J13" s="6"/>
       <c r="K13" s="6"/>
       <c r="L13" s="6"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>7</v>
-      </c>
+      <c r="M13" s="5"/>
+      <c r="N13" s="6"/>
+      <c r="O13" s="6"/>
+      <c r="P13" s="6"/>
+      <c r="Q13" s="6"/>
+      <c r="R13" s="6"/>
+      <c r="S13" s="6"/>
+      <c r="T13" s="6"/>
+      <c r="U13" s="6"/>
+      <c r="V13" s="6"/>
+      <c r="W13" s="6"/>
+      <c r="X13" s="6"/>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A14" s="10"/>
+      <c r="B14" s="10"/>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
@@ -1318,8 +1576,21 @@
       <c r="J14" s="6"/>
       <c r="K14" s="6"/>
       <c r="L14" s="6"/>
-    </row>
-    <row r="15" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M14" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="O14" s="6"/>
+      <c r="P14" s="6"/>
+      <c r="Q14" s="6"/>
+      <c r="R14" s="6"/>
+      <c r="S14" s="6"/>
+      <c r="T14" s="6"/>
+      <c r="U14" s="6"/>
+      <c r="V14" s="6"/>
+      <c r="W14" s="6"/>
+      <c r="X14" s="6"/>
+    </row>
+    <row r="15" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
@@ -1330,8 +1601,20 @@
       <c r="J15" s="6"/>
       <c r="K15" s="6"/>
       <c r="L15" s="6"/>
-    </row>
-    <row r="16" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M15" s="6"/>
+      <c r="N15" s="6"/>
+      <c r="O15" s="6"/>
+      <c r="P15" s="6"/>
+      <c r="Q15" s="6"/>
+      <c r="R15" s="6"/>
+      <c r="S15" s="6"/>
+      <c r="T15" s="6"/>
+      <c r="U15" s="6"/>
+      <c r="V15" s="6"/>
+      <c r="W15" s="6"/>
+      <c r="X15" s="6"/>
+    </row>
+    <row r="16" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
@@ -1342,8 +1625,22 @@
       <c r="J16" s="6"/>
       <c r="K16" s="6"/>
       <c r="L16" s="6"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M16" s="6"/>
+      <c r="N16" s="6"/>
+      <c r="O16" s="6"/>
+      <c r="P16" s="6"/>
+      <c r="Q16" s="6"/>
+      <c r="R16" s="6"/>
+      <c r="S16" s="6"/>
+      <c r="T16" s="6"/>
+      <c r="U16" s="6"/>
+      <c r="V16" s="6"/>
+      <c r="W16" s="6"/>
+      <c r="X16" s="6"/>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A17" s="10"/>
+      <c r="B17" s="10"/>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
@@ -1354,11 +1651,24 @@
       <c r="J17" s="6"/>
       <c r="K17" s="6"/>
       <c r="L17" s="6"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>8</v>
-      </c>
+      <c r="M17" s="6"/>
+      <c r="N17" s="6"/>
+      <c r="O17" s="6"/>
+      <c r="P17" s="6"/>
+      <c r="Q17" s="6"/>
+      <c r="R17" s="6"/>
+      <c r="S17" s="6"/>
+      <c r="T17" s="6"/>
+      <c r="U17" s="6"/>
+      <c r="V17" s="6"/>
+      <c r="W17" s="6"/>
+      <c r="X17" s="6"/>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A18" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" s="10"/>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
@@ -1369,8 +1679,20 @@
       <c r="J18" s="6"/>
       <c r="K18" s="6"/>
       <c r="L18" s="6"/>
-    </row>
-    <row r="19" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M18" s="6"/>
+      <c r="N18" s="6"/>
+      <c r="O18" s="6"/>
+      <c r="P18" s="6"/>
+      <c r="Q18" s="6"/>
+      <c r="R18" s="6"/>
+      <c r="S18" s="6"/>
+      <c r="T18" s="6"/>
+      <c r="U18" s="6"/>
+      <c r="V18" s="6"/>
+      <c r="W18" s="6"/>
+      <c r="X18" s="6"/>
+    </row>
+    <row r="19" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
@@ -1381,390 +1703,736 @@
       <c r="J19" s="6"/>
       <c r="K19" s="6"/>
       <c r="L19" s="6"/>
-    </row>
-    <row r="20" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="6"/>
-      <c r="K20" s="6"/>
-      <c r="L20" s="6"/>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
-      <c r="J22" s="3"/>
-      <c r="K22" s="3"/>
-      <c r="L22" s="3"/>
-    </row>
-    <row r="23" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="5"/>
+      <c r="M19" s="6"/>
+      <c r="N19" s="6"/>
+      <c r="O19" s="6"/>
+      <c r="P19" s="6"/>
+      <c r="Q19" s="6"/>
+      <c r="R19" s="6"/>
+      <c r="S19" s="6"/>
+      <c r="T19" s="6"/>
+      <c r="U19" s="6"/>
+      <c r="V19" s="6"/>
+      <c r="W19" s="6"/>
+      <c r="X19" s="6"/>
+    </row>
+    <row r="20" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="M20" s="6"/>
+      <c r="N20" s="6"/>
+      <c r="O20" s="6"/>
+      <c r="P20" s="6"/>
+      <c r="Q20" s="6"/>
+      <c r="R20" s="6"/>
+      <c r="S20" s="6"/>
+      <c r="T20" s="6"/>
+      <c r="U20" s="6"/>
+      <c r="V20" s="6"/>
+      <c r="W20" s="6"/>
+      <c r="X20" s="6"/>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A21" s="10"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
+      <c r="L21" s="6"/>
+      <c r="M21" s="6"/>
+      <c r="N21" s="6"/>
+      <c r="O21" s="6"/>
+      <c r="P21" s="6"/>
+      <c r="Q21" s="6"/>
+      <c r="R21" s="6"/>
+      <c r="S21" s="6"/>
+      <c r="T21" s="6"/>
+      <c r="U21" s="6"/>
+      <c r="V21" s="6"/>
+      <c r="W21" s="6"/>
+      <c r="X21" s="6"/>
+    </row>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A22" s="5"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
+      <c r="K22" s="6"/>
+      <c r="L22" s="6"/>
+      <c r="M22" s="5"/>
+      <c r="N22" s="6"/>
+      <c r="O22" s="6"/>
+      <c r="P22" s="6"/>
+      <c r="Q22" s="6"/>
+      <c r="R22" s="6"/>
+      <c r="S22" s="6"/>
+      <c r="T22" s="6"/>
+      <c r="U22" s="6"/>
+      <c r="V22" s="6"/>
+      <c r="W22" s="6"/>
+      <c r="X22" s="6"/>
+    </row>
+    <row r="23" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="6"/>
       <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C24" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D24" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="E24" s="21"/>
-      <c r="F24" s="21" t="s">
-        <v>11</v>
-      </c>
-      <c r="G24" s="21"/>
-      <c r="H24" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="I24" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="J24" s="21"/>
-      <c r="K24" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="L24" s="21"/>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C25" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D25" s="17"/>
-      <c r="E25" s="17"/>
-      <c r="F25" s="17"/>
-      <c r="G25" s="17"/>
-      <c r="H25" s="14"/>
-      <c r="I25" s="17"/>
-      <c r="J25" s="17"/>
-      <c r="K25" s="17"/>
-      <c r="L25" s="17"/>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C26" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D26" s="17"/>
-      <c r="E26" s="17"/>
-      <c r="F26" s="17"/>
-      <c r="G26" s="17"/>
-      <c r="H26" s="14"/>
-      <c r="I26" s="17"/>
-      <c r="J26" s="17"/>
-      <c r="K26" s="17"/>
-      <c r="L26" s="17"/>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C27" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D27" s="17"/>
-      <c r="E27" s="17"/>
-      <c r="F27" s="17"/>
-      <c r="G27" s="17"/>
-      <c r="H27" s="14"/>
-      <c r="I27" s="17"/>
-      <c r="J27" s="17"/>
-      <c r="K27" s="17"/>
-      <c r="L27" s="17"/>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C28" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D28" s="17"/>
-      <c r="E28" s="17"/>
-      <c r="F28" s="17"/>
-      <c r="G28" s="17"/>
-      <c r="H28" s="14"/>
-      <c r="I28" s="17"/>
-      <c r="J28" s="17"/>
-      <c r="K28" s="17"/>
-      <c r="L28" s="17"/>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
-      <c r="I30" s="3"/>
-      <c r="J30" s="3"/>
-      <c r="K30" s="3"/>
-      <c r="L30" s="3"/>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>18</v>
-      </c>
+      <c r="C23" s="16"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="20"/>
+      <c r="H23" s="17"/>
+      <c r="I23" s="20"/>
+      <c r="J23" s="20"/>
+      <c r="K23" s="20"/>
+      <c r="L23" s="20"/>
+      <c r="M23" s="5"/>
+      <c r="N23" s="6"/>
+      <c r="O23" s="6"/>
+      <c r="P23" s="6"/>
+      <c r="Q23" s="6"/>
+      <c r="R23" s="6"/>
+      <c r="S23" s="6"/>
+      <c r="T23" s="6"/>
+      <c r="U23" s="6"/>
+      <c r="V23" s="6"/>
+      <c r="W23" s="6"/>
+      <c r="X23" s="6"/>
+    </row>
+    <row r="24" spans="1:24" ht="16" x14ac:dyDescent="0.45">
+      <c r="A24" s="6"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="19"/>
+      <c r="F24" s="19"/>
+      <c r="G24" s="19"/>
+      <c r="H24" s="15"/>
+      <c r="I24" s="19"/>
+      <c r="J24" s="19"/>
+      <c r="K24" s="19"/>
+      <c r="L24" s="19"/>
+      <c r="M24" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="N24" s="3"/>
+      <c r="O24" s="3"/>
+      <c r="P24" s="3"/>
+      <c r="Q24" s="3"/>
+      <c r="R24" s="3"/>
+      <c r="S24" s="3"/>
+      <c r="T24" s="3"/>
+      <c r="U24" s="3"/>
+      <c r="V24" s="3"/>
+      <c r="W24" s="3"/>
+      <c r="X24" s="3"/>
+    </row>
+    <row r="25" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A25" s="10"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="19"/>
+      <c r="F25" s="19"/>
+      <c r="G25" s="19"/>
+      <c r="H25" s="15"/>
+      <c r="I25" s="19"/>
+      <c r="J25" s="19"/>
+      <c r="K25" s="19"/>
+      <c r="L25" s="19"/>
+      <c r="M25" s="5"/>
+      <c r="N25" s="6"/>
+      <c r="O25" s="6"/>
+      <c r="P25" s="6"/>
+      <c r="Q25" s="6"/>
+      <c r="R25" s="6"/>
+      <c r="S25" s="6"/>
+      <c r="T25" s="6"/>
+      <c r="U25" s="6"/>
+      <c r="V25" s="6"/>
+      <c r="W25" s="6"/>
+      <c r="X25" s="6"/>
+    </row>
+    <row r="26" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A26" s="6"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="19"/>
+      <c r="F26" s="19"/>
+      <c r="G26" s="19"/>
+      <c r="H26" s="15"/>
+      <c r="I26" s="19"/>
+      <c r="J26" s="19"/>
+      <c r="K26" s="19"/>
+      <c r="L26" s="19"/>
+      <c r="M26" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="O26" s="6"/>
+      <c r="P26" s="6"/>
+      <c r="Q26" s="6"/>
+      <c r="R26" s="6"/>
+      <c r="S26" s="6"/>
+      <c r="T26" s="6"/>
+      <c r="U26" s="6"/>
+      <c r="V26" s="6"/>
+      <c r="W26" s="6"/>
+      <c r="X26" s="6"/>
+    </row>
+    <row r="27" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A27" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="19"/>
+      <c r="E27" s="19"/>
+      <c r="F27" s="19"/>
+      <c r="G27" s="19"/>
+      <c r="H27" s="15"/>
+      <c r="I27" s="19"/>
+      <c r="J27" s="19"/>
+      <c r="K27" s="19"/>
+      <c r="L27" s="19"/>
+      <c r="O27" s="6"/>
+      <c r="P27" s="6"/>
+      <c r="Q27" s="6"/>
+      <c r="R27" s="6"/>
+      <c r="S27" s="6"/>
+      <c r="T27" s="6"/>
+      <c r="U27" s="6"/>
+      <c r="V27" s="6"/>
+      <c r="W27" s="6"/>
+      <c r="X27" s="6"/>
+    </row>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A28" s="6"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="6"/>
+      <c r="J28" s="6"/>
+      <c r="K28" s="6"/>
+      <c r="L28" s="6"/>
+      <c r="O28" s="6"/>
+      <c r="P28" s="6"/>
+      <c r="Q28" s="6"/>
+      <c r="R28" s="6"/>
+      <c r="S28" s="6"/>
+      <c r="T28" s="6"/>
+      <c r="U28" s="6"/>
+      <c r="V28" s="6"/>
+      <c r="W28" s="6"/>
+      <c r="X28" s="6"/>
+    </row>
+    <row r="29" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A29" s="5"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
+      <c r="I29" s="6"/>
+      <c r="J29" s="6"/>
+      <c r="K29" s="6"/>
+      <c r="L29" s="6"/>
+      <c r="O29" s="6"/>
+      <c r="P29" s="6"/>
+      <c r="Q29" s="6"/>
+      <c r="R29" s="6"/>
+      <c r="S29" s="6"/>
+      <c r="T29" s="6"/>
+      <c r="U29" s="6"/>
+      <c r="V29" s="6"/>
+      <c r="W29" s="6"/>
+      <c r="X29" s="6"/>
+    </row>
+    <row r="30" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A30" s="6"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="6"/>
+      <c r="I30" s="6"/>
+      <c r="J30" s="6"/>
+      <c r="K30" s="6"/>
+      <c r="L30" s="6"/>
+      <c r="O30" s="6"/>
+      <c r="P30" s="6"/>
+      <c r="Q30" s="6"/>
+      <c r="R30" s="6"/>
+      <c r="S30" s="6"/>
+      <c r="T30" s="6"/>
+      <c r="U30" s="6"/>
+      <c r="V30" s="6"/>
+      <c r="W30" s="6"/>
+      <c r="X30" s="6"/>
+    </row>
+    <row r="31" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A31" s="6"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
+      <c r="I31" s="6"/>
+      <c r="J31" s="6"/>
+      <c r="K31" s="6"/>
+      <c r="L31" s="6"/>
+      <c r="O31" s="6"/>
+      <c r="P31" s="6"/>
+      <c r="Q31" s="6"/>
+      <c r="R31" s="6"/>
+      <c r="S31" s="6"/>
+      <c r="T31" s="6"/>
+      <c r="U31" s="6"/>
+      <c r="V31" s="6"/>
+      <c r="W31" s="6"/>
+      <c r="X31" s="6"/>
+    </row>
+    <row r="32" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A32" s="6"/>
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>
-      <c r="E32" t="s">
-        <v>19</v>
-      </c>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
       <c r="G32" s="6"/>
       <c r="H32" s="6"/>
       <c r="I32" s="6"/>
       <c r="J32" s="6"/>
       <c r="K32" s="6"/>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
+      <c r="L32" s="6"/>
+      <c r="O32" s="6"/>
+      <c r="P32" s="6"/>
+      <c r="Q32" s="6"/>
+      <c r="R32" s="6"/>
+      <c r="S32" s="6"/>
+      <c r="T32" s="6"/>
+      <c r="U32" s="6"/>
+      <c r="V32" s="6"/>
+      <c r="W32" s="6"/>
+      <c r="X32" s="6"/>
+    </row>
+    <row r="33" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A33" s="5"/>
+      <c r="B33" s="6"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="6"/>
+      <c r="I33" s="6"/>
+      <c r="J33" s="6"/>
+      <c r="K33" s="6"/>
+      <c r="L33" s="6"/>
+      <c r="M33" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="O33" s="6"/>
+      <c r="P33" s="6"/>
+      <c r="Q33" s="6"/>
+      <c r="R33" s="6"/>
+      <c r="S33" s="6"/>
+      <c r="T33" s="6"/>
+      <c r="U33" s="6"/>
+      <c r="V33" s="6"/>
+      <c r="W33" s="6"/>
+      <c r="X33" s="6"/>
+    </row>
+    <row r="34" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A34" s="10"/>
+      <c r="B34" s="10"/>
+      <c r="C34" s="10"/>
+      <c r="D34" s="10"/>
+      <c r="E34" s="10"/>
+      <c r="F34" s="10"/>
+      <c r="G34" s="10"/>
+      <c r="H34" s="10"/>
+      <c r="L34" s="10"/>
+      <c r="O34" s="6"/>
+      <c r="P34" s="6"/>
+      <c r="Q34" s="6"/>
+      <c r="R34" s="6"/>
+      <c r="S34" s="6"/>
+      <c r="T34" s="6"/>
+      <c r="U34" s="6"/>
+      <c r="V34" s="6"/>
+      <c r="W34" s="6"/>
+      <c r="X34" s="6"/>
+    </row>
+    <row r="35" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A35" s="10"/>
+      <c r="B35" s="10"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="10"/>
+      <c r="E35" s="10"/>
+      <c r="F35" s="10"/>
+      <c r="G35" s="10"/>
+      <c r="H35" s="10"/>
+      <c r="L35" s="10"/>
+      <c r="O35" s="6"/>
+      <c r="P35" s="6"/>
+      <c r="Q35" s="6"/>
+      <c r="R35" s="6"/>
+      <c r="S35" s="6"/>
+      <c r="T35" s="6"/>
+      <c r="U35" s="6"/>
+      <c r="V35" s="6"/>
+      <c r="W35" s="6"/>
+      <c r="X35" s="6"/>
+    </row>
+    <row r="36" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A36" s="10"/>
+      <c r="B36" s="10"/>
+      <c r="C36" s="10"/>
+      <c r="D36" s="10"/>
+      <c r="E36" s="10"/>
+      <c r="F36" s="10"/>
+      <c r="G36" s="10"/>
+      <c r="H36" s="10"/>
+      <c r="L36" s="10"/>
+      <c r="O36" s="6"/>
+      <c r="P36" s="6"/>
+      <c r="Q36" s="6"/>
+      <c r="R36" s="6"/>
+      <c r="S36" s="6"/>
+      <c r="T36" s="6"/>
+      <c r="U36" s="6"/>
+      <c r="V36" s="6"/>
+      <c r="W36" s="6"/>
+      <c r="X36" s="6"/>
+    </row>
+    <row r="37" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A37" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B37" s="3"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="3"/>
+      <c r="H37" s="3"/>
+      <c r="I37" s="3"/>
+      <c r="J37" s="3"/>
+      <c r="K37" s="3"/>
+      <c r="L37" s="3"/>
+    </row>
+    <row r="38" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A38" s="5"/>
+      <c r="B38" s="6"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6"/>
+      <c r="F38" s="6"/>
+      <c r="G38" s="6"/>
+      <c r="H38" s="10"/>
+      <c r="L38" s="10"/>
+      <c r="O38" s="6"/>
+      <c r="P38" s="6"/>
+      <c r="Q38" s="6"/>
+      <c r="R38" s="6"/>
+      <c r="S38" s="6"/>
+      <c r="T38" s="6"/>
+      <c r="U38" s="6"/>
+      <c r="V38" s="6"/>
+      <c r="W38" s="6"/>
+      <c r="X38" s="6"/>
+    </row>
+    <row r="39" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A39" s="10"/>
+      <c r="B39" s="10"/>
+      <c r="C39" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D39" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="E39" s="30"/>
+      <c r="F39" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="G39" s="30"/>
+      <c r="H39" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="I39" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="J39" s="30"/>
+      <c r="K39" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="L39" s="30"/>
+      <c r="O39" s="6"/>
+      <c r="P39" s="6"/>
+      <c r="Q39" s="6"/>
+      <c r="R39" s="6"/>
+      <c r="S39" s="6"/>
+      <c r="T39" s="6"/>
+      <c r="U39" s="6"/>
+      <c r="V39" s="6"/>
+      <c r="W39" s="6"/>
+      <c r="X39" s="6"/>
+    </row>
+    <row r="40" spans="1:24" ht="16" x14ac:dyDescent="0.45">
+      <c r="A40" s="10"/>
+      <c r="B40" s="10"/>
+      <c r="C40" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D40" s="31"/>
+      <c r="E40" s="32"/>
+      <c r="F40" s="31"/>
+      <c r="G40" s="32"/>
+      <c r="H40" s="11"/>
+      <c r="I40" s="31"/>
+      <c r="J40" s="32"/>
+      <c r="K40" s="31"/>
+      <c r="L40" s="32"/>
+      <c r="M40" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="O40" s="16"/>
+      <c r="P40" s="20"/>
+      <c r="Q40" s="20"/>
+      <c r="R40" s="20"/>
+      <c r="S40" s="20"/>
+      <c r="T40" s="17"/>
+      <c r="U40" s="20"/>
+      <c r="V40" s="20"/>
+      <c r="W40" s="20"/>
+      <c r="X40" s="20"/>
+    </row>
+    <row r="41" spans="1:24" s="10" customFormat="1" ht="16" x14ac:dyDescent="0.45">
+      <c r="C41" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D41" s="31"/>
+      <c r="E41" s="32"/>
+      <c r="F41" s="31"/>
+      <c r="G41" s="32"/>
+      <c r="H41" s="11"/>
+      <c r="I41" s="31"/>
+      <c r="J41" s="32"/>
+      <c r="K41" s="31"/>
+      <c r="L41" s="32"/>
+      <c r="O41" s="18"/>
+      <c r="P41" s="19"/>
+      <c r="Q41" s="19"/>
+      <c r="R41" s="19"/>
+      <c r="S41" s="19"/>
+      <c r="T41" s="15"/>
+      <c r="U41" s="19"/>
+      <c r="V41" s="19"/>
+      <c r="W41" s="19"/>
+      <c r="X41" s="19"/>
+    </row>
+    <row r="42" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C42" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D42" s="31"/>
+      <c r="E42" s="32"/>
+      <c r="F42" s="31"/>
+      <c r="G42" s="32"/>
+      <c r="H42" s="11"/>
+      <c r="I42" s="31"/>
+      <c r="J42" s="32"/>
+      <c r="K42" s="31"/>
+      <c r="L42" s="32"/>
+      <c r="O42" s="6"/>
+      <c r="P42" s="19"/>
+      <c r="Q42" s="19"/>
+      <c r="R42" s="19"/>
+      <c r="S42" s="19"/>
+      <c r="T42" s="15"/>
+      <c r="U42" s="19"/>
+      <c r="V42" s="19"/>
+      <c r="W42" s="19"/>
+      <c r="X42" s="19"/>
+    </row>
+    <row r="43" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C43" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D43" s="31"/>
+      <c r="E43" s="32"/>
+      <c r="F43" s="31"/>
+      <c r="G43" s="32"/>
+      <c r="H43" s="11"/>
+      <c r="I43" s="31"/>
+      <c r="J43" s="32"/>
+      <c r="K43" s="31"/>
+      <c r="L43" s="32"/>
+      <c r="O43" s="6"/>
+      <c r="P43" s="19"/>
+      <c r="Q43" s="19"/>
+      <c r="R43" s="19"/>
+      <c r="S43" s="19"/>
+      <c r="T43" s="15"/>
+      <c r="U43" s="19"/>
+      <c r="V43" s="19"/>
+      <c r="W43" s="19"/>
+      <c r="X43" s="19"/>
+    </row>
+    <row r="44" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="O44" s="6"/>
+      <c r="P44" s="19"/>
+      <c r="Q44" s="19"/>
+      <c r="R44" s="19"/>
+      <c r="S44" s="19"/>
+      <c r="T44" s="15"/>
+      <c r="U44" s="19"/>
+      <c r="V44" s="19"/>
+      <c r="W44" s="19"/>
+      <c r="X44" s="19"/>
+    </row>
+    <row r="45" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B45" s="3"/>
+      <c r="C45" s="3"/>
+      <c r="D45" s="3"/>
+      <c r="E45" s="3"/>
+      <c r="F45" s="3"/>
+      <c r="G45" s="3"/>
+      <c r="H45" s="3"/>
+      <c r="I45" s="3"/>
+      <c r="J45" s="3"/>
+      <c r="K45" s="3"/>
+      <c r="L45" s="3"/>
+    </row>
+    <row r="46" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A46" s="10"/>
+      <c r="B46" s="10"/>
+      <c r="C46" s="10"/>
+      <c r="D46" s="10"/>
+      <c r="E46" s="10"/>
+      <c r="F46" s="10"/>
+      <c r="G46" s="10"/>
+      <c r="H46" s="10"/>
+      <c r="L46" s="10"/>
+    </row>
+    <row r="47" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A47" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B47" s="6"/>
+      <c r="C47" s="6"/>
+      <c r="D47" s="10"/>
+      <c r="E47" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="F47" s="10"/>
+      <c r="G47" s="6"/>
+      <c r="H47" s="6"/>
+      <c r="I47" s="6"/>
+      <c r="J47" s="6"/>
+      <c r="K47" s="6"/>
+      <c r="L47" s="10"/>
+      <c r="M47" s="10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="48" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="49" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A49" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
-      <c r="E34" s="3"/>
-      <c r="F34" s="3"/>
-      <c r="G34" s="3"/>
-      <c r="H34" s="3"/>
-      <c r="I34" s="3"/>
-      <c r="J34" s="3"/>
-      <c r="K34" s="3"/>
-      <c r="L34" s="3"/>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="B49" s="3"/>
+      <c r="C49" s="3"/>
+      <c r="D49" s="3"/>
+      <c r="E49" s="3"/>
+      <c r="F49" s="3"/>
+      <c r="G49" s="3"/>
+      <c r="H49" s="3"/>
+      <c r="I49" s="3"/>
+      <c r="J49" s="3"/>
+      <c r="K49" s="3"/>
+      <c r="L49" s="3"/>
+    </row>
+    <row r="50" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A50" s="10"/>
+      <c r="B50" s="10"/>
+      <c r="C50" s="10"/>
+      <c r="D50" s="10"/>
+      <c r="E50" s="10"/>
+      <c r="F50" s="10"/>
+      <c r="G50" s="10"/>
+      <c r="H50" s="10"/>
+      <c r="L50" s="10"/>
+    </row>
+    <row r="51" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A51" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C36" s="6"/>
-      <c r="E36" t="s">
+      <c r="B51" s="10"/>
+      <c r="C51" s="6"/>
+      <c r="D51" s="10"/>
+      <c r="E51" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="I36" s="6"/>
-      <c r="J36" s="6"/>
-      <c r="K36" s="6"/>
-      <c r="L36" s="6"/>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>25</v>
-      </c>
-      <c r="C37" s="6"/>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A39" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B39" s="3"/>
-      <c r="C39" s="3"/>
-      <c r="D39" s="3"/>
-      <c r="E39" s="3"/>
-      <c r="F39" s="3"/>
-      <c r="G39" s="3"/>
-      <c r="H39" s="3"/>
-      <c r="I39" s="3"/>
-      <c r="J39" s="3"/>
-      <c r="K39" s="3"/>
-      <c r="L39" s="3"/>
-    </row>
-    <row r="41" spans="1:12" s="11" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C41" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D41" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="E41" s="19"/>
-      <c r="F41" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="G41" s="19"/>
-      <c r="H41" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="I41" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="J41" s="22"/>
-      <c r="K41" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="L41" s="23"/>
-    </row>
-    <row r="42" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C42" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="D42" s="20"/>
-      <c r="E42" s="20"/>
-      <c r="F42" s="17"/>
-      <c r="G42" s="17"/>
-      <c r="H42" s="10"/>
-      <c r="I42" s="17"/>
-      <c r="J42" s="17"/>
-      <c r="K42" s="17"/>
-      <c r="L42" s="17"/>
-    </row>
-    <row r="43" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C43" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="D43" s="17"/>
-      <c r="E43" s="17"/>
-      <c r="F43" s="17"/>
-      <c r="G43" s="17"/>
-      <c r="H43" s="10"/>
-      <c r="I43" s="17"/>
-      <c r="J43" s="17"/>
-      <c r="K43" s="17"/>
-      <c r="L43" s="17"/>
-    </row>
-    <row r="44" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C44" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="D44" s="17"/>
-      <c r="E44" s="17"/>
-      <c r="F44" s="17"/>
-      <c r="G44" s="17"/>
-      <c r="H44" s="10"/>
-      <c r="I44" s="17"/>
-      <c r="J44" s="17"/>
-      <c r="K44" s="17"/>
-      <c r="L44" s="17"/>
-    </row>
-    <row r="45" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C45" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="D45" s="17"/>
-      <c r="E45" s="17"/>
-      <c r="F45" s="17"/>
-      <c r="G45" s="17"/>
-      <c r="H45" s="10"/>
-      <c r="I45" s="17"/>
-      <c r="J45" s="17"/>
-      <c r="K45" s="17"/>
-      <c r="L45" s="17"/>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B46" s="11"/>
-      <c r="C46" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="D46" s="17"/>
-      <c r="E46" s="17"/>
-      <c r="F46" s="17"/>
-      <c r="G46" s="17"/>
-      <c r="H46" s="10"/>
-      <c r="I46" s="17"/>
-      <c r="J46" s="17"/>
-      <c r="K46" s="17"/>
-      <c r="L46" s="17"/>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C47" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="D47" s="17"/>
-      <c r="E47" s="17"/>
-      <c r="F47" s="17"/>
-      <c r="G47" s="17"/>
-      <c r="H47" s="10"/>
-      <c r="I47" s="17"/>
-      <c r="J47" s="17"/>
-      <c r="K47" s="17"/>
-      <c r="L47" s="17"/>
-    </row>
-    <row r="48" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C48" s="24"/>
-      <c r="D48" s="25"/>
-      <c r="E48" s="25"/>
-      <c r="F48" s="25"/>
-      <c r="G48" s="25"/>
-      <c r="H48" s="6"/>
-      <c r="I48" s="25"/>
-      <c r="J48" s="25"/>
-      <c r="K48" s="25"/>
-      <c r="L48" s="25"/>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A50" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B50" s="3"/>
-      <c r="C50" s="3"/>
-      <c r="D50" s="3"/>
-      <c r="E50" s="3"/>
-      <c r="F50" s="3"/>
-      <c r="G50" s="3"/>
-      <c r="H50" s="3"/>
-      <c r="I50" s="3"/>
-      <c r="J50" s="3"/>
-      <c r="K50" s="3"/>
-      <c r="L50" s="3"/>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A51" s="5"/>
-      <c r="B51" s="6"/>
-      <c r="C51" s="6"/>
-      <c r="D51" s="6"/>
-      <c r="E51" s="6"/>
-      <c r="F51" s="6"/>
-      <c r="G51" s="6"/>
-      <c r="H51" s="6"/>
+      <c r="F51" s="10"/>
+      <c r="G51" s="10"/>
+      <c r="H51" s="10"/>
       <c r="I51" s="6"/>
       <c r="J51" s="6"/>
       <c r="K51" s="6"/>
       <c r="L51" s="6"/>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A52" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B52" s="11"/>
+    <row r="52" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A52" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B52" s="10"/>
       <c r="C52" s="6"/>
-      <c r="D52" s="6"/>
-      <c r="E52" s="6"/>
-      <c r="F52" s="6"/>
-      <c r="G52" s="6"/>
-      <c r="H52" s="6"/>
-      <c r="I52" s="6"/>
-      <c r="J52" s="6"/>
-      <c r="K52" s="6"/>
-      <c r="L52" s="6"/>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A53" s="11"/>
-      <c r="B53" s="11"/>
-      <c r="C53" s="6"/>
-      <c r="D53" s="6"/>
-      <c r="E53" s="6"/>
-      <c r="F53" s="6"/>
-      <c r="G53" s="6"/>
-      <c r="H53" s="6"/>
-      <c r="I53" s="6"/>
-      <c r="J53" s="6"/>
-      <c r="K53" s="6"/>
-      <c r="L53" s="6"/>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A54" s="11"/>
-      <c r="B54" s="11"/>
+      <c r="D52" s="10"/>
+      <c r="E52" s="10"/>
+      <c r="F52" s="10"/>
+      <c r="G52" s="10"/>
+      <c r="H52" s="10"/>
+      <c r="L52" s="10"/>
+    </row>
+    <row r="53" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="O53" s="6"/>
+      <c r="P53" s="6"/>
+      <c r="Q53" s="6"/>
+      <c r="R53" s="6"/>
+      <c r="S53" s="6"/>
+      <c r="T53" s="6"/>
+      <c r="U53" s="6"/>
+      <c r="V53" s="6"/>
+      <c r="W53" s="6"/>
+      <c r="X53" s="6"/>
+    </row>
+    <row r="54" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A54" s="10"/>
+      <c r="B54" s="10"/>
       <c r="C54" s="6"/>
       <c r="D54" s="6"/>
       <c r="E54" s="6"/>
@@ -1775,58 +2443,75 @@
       <c r="J54" s="6"/>
       <c r="K54" s="6"/>
       <c r="L54" s="6"/>
+      <c r="O54" s="6"/>
+      <c r="P54" s="6"/>
+      <c r="Q54" s="6"/>
+      <c r="R54" s="6"/>
+      <c r="S54" s="6"/>
+      <c r="T54" s="6"/>
+      <c r="U54" s="6"/>
+      <c r="V54" s="6"/>
+      <c r="W54" s="6"/>
+      <c r="X54" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="49">
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="I28:J28"/>
-    <mergeCell ref="I27:J27"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="I24:J24"/>
-    <mergeCell ref="K28:L28"/>
-    <mergeCell ref="K27:L27"/>
-    <mergeCell ref="K26:L26"/>
-    <mergeCell ref="K25:L25"/>
-    <mergeCell ref="K24:L24"/>
+  <mergeCells count="56">
+    <mergeCell ref="I43:J43"/>
     <mergeCell ref="I42:J42"/>
     <mergeCell ref="I41:J41"/>
-    <mergeCell ref="K47:L47"/>
-    <mergeCell ref="K46:L46"/>
-    <mergeCell ref="K45:L45"/>
-    <mergeCell ref="K44:L44"/>
+    <mergeCell ref="I40:J40"/>
+    <mergeCell ref="I39:J39"/>
     <mergeCell ref="K43:L43"/>
     <mergeCell ref="K42:L42"/>
     <mergeCell ref="K41:L41"/>
-    <mergeCell ref="I47:J47"/>
-    <mergeCell ref="I46:J46"/>
-    <mergeCell ref="I45:J45"/>
-    <mergeCell ref="I44:J44"/>
-    <mergeCell ref="I43:J43"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="K40:L40"/>
+    <mergeCell ref="K39:L39"/>
     <mergeCell ref="D43:E43"/>
-    <mergeCell ref="F47:G47"/>
-    <mergeCell ref="F46:G46"/>
-    <mergeCell ref="F45:G45"/>
-    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="F40:G40"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="F42:G42"/>
     <mergeCell ref="F43:G43"/>
     <mergeCell ref="B1:B2"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="D41:E41"/>
     <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="R3:S3"/>
+    <mergeCell ref="U3:V3"/>
+    <mergeCell ref="W3:X3"/>
+    <mergeCell ref="P4:Q4"/>
+    <mergeCell ref="R4:S4"/>
+    <mergeCell ref="U4:V4"/>
+    <mergeCell ref="W4:X4"/>
+    <mergeCell ref="P5:Q5"/>
+    <mergeCell ref="R5:S5"/>
+    <mergeCell ref="U5:V5"/>
+    <mergeCell ref="W5:X5"/>
+    <mergeCell ref="P6:Q6"/>
+    <mergeCell ref="R6:S6"/>
+    <mergeCell ref="U6:V6"/>
+    <mergeCell ref="W6:X6"/>
+    <mergeCell ref="W9:X9"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="R7:S7"/>
+    <mergeCell ref="U7:V7"/>
+    <mergeCell ref="W7:X7"/>
+    <mergeCell ref="P8:Q8"/>
+    <mergeCell ref="R8:S8"/>
+    <mergeCell ref="U8:V8"/>
+    <mergeCell ref="W8:X8"/>
+    <mergeCell ref="N8:O8"/>
+    <mergeCell ref="N9:O9"/>
+    <mergeCell ref="P9:Q9"/>
+    <mergeCell ref="R9:S9"/>
+    <mergeCell ref="U9:V9"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="N7:O7"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25297619047619047" top="0.25297619047619047" bottom="0.25297619047619047" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Fixes #30 : champs RGPD obligatoires + correction intitulé RGPD dans le PDF
</commit_message>
<xml_diff>
--- a/public/dependencies/includes/Fiche info projet.xlsx
+++ b/public/dependencies/includes/Fiche info projet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\dev-requests\public\dependencies\includes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{0C7746AF-5078-4855-A84A-3CAA81A41512}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A8B182F-6307-4351-9ECC-A2279BB6472B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="150" windowWidth="24920" windowHeight="12080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="44">
   <si>
     <t>DevReq</t>
   </si>
@@ -150,6 +150,9 @@
   </si>
   <si>
     <t>Impact</t>
+  </si>
+  <si>
+    <t>Informations RGPD</t>
   </si>
 </sst>
 </file>
@@ -716,14 +719,20 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -732,25 +741,19 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="78">
@@ -1225,7 +1228,7 @@
   <dimension ref="A1:X54"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScale="55" zoomScaleNormal="70" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="55" workbookViewId="0">
-      <selection activeCell="I39" sqref="I39:J39"/>
+      <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1247,7 +1250,7 @@
   <sheetData>
     <row r="1" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="25" t="s">
         <v>0</v>
       </c>
       <c r="M1" s="4" t="s">
@@ -1267,7 +1270,7 @@
     </row>
     <row r="2" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
-      <c r="B2" s="28"/>
+      <c r="B2" s="25"/>
       <c r="D2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1281,29 +1284,29 @@
       <c r="L2" s="6"/>
     </row>
     <row r="3" spans="1:24" ht="39" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="N3" s="21" t="s">
+      <c r="N3" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="O3" s="21"/>
-      <c r="P3" s="24" t="s">
+      <c r="O3" s="28"/>
+      <c r="P3" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="Q3" s="25"/>
-      <c r="R3" s="24" t="s">
+      <c r="Q3" s="27"/>
+      <c r="R3" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="S3" s="25"/>
+      <c r="S3" s="27"/>
       <c r="T3" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="U3" s="21" t="s">
+      <c r="U3" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="V3" s="21"/>
-      <c r="W3" s="26" t="s">
+      <c r="V3" s="28"/>
+      <c r="W3" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="X3" s="26"/>
+      <c r="X3" s="29"/>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A4" s="10" t="s">
@@ -1322,19 +1325,19 @@
       <c r="J4" s="6"/>
       <c r="K4" s="6"/>
       <c r="L4" s="6"/>
-      <c r="N4" s="22" t="s">
+      <c r="N4" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="O4" s="22"/>
-      <c r="P4" s="27"/>
-      <c r="Q4" s="27"/>
-      <c r="R4" s="23"/>
-      <c r="S4" s="23"/>
+      <c r="O4" s="32"/>
+      <c r="P4" s="30"/>
+      <c r="Q4" s="30"/>
+      <c r="R4" s="31"/>
+      <c r="S4" s="31"/>
       <c r="T4" s="9"/>
-      <c r="U4" s="23"/>
-      <c r="V4" s="23"/>
-      <c r="W4" s="23"/>
-      <c r="X4" s="23"/>
+      <c r="U4" s="31"/>
+      <c r="V4" s="31"/>
+      <c r="W4" s="31"/>
+      <c r="X4" s="31"/>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A5" s="10" t="s">
@@ -1353,19 +1356,19 @@
       <c r="J5" s="6"/>
       <c r="K5" s="6"/>
       <c r="L5" s="6"/>
-      <c r="N5" s="22" t="s">
+      <c r="N5" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="O5" s="22"/>
-      <c r="P5" s="23"/>
-      <c r="Q5" s="23"/>
-      <c r="R5" s="23"/>
-      <c r="S5" s="23"/>
+      <c r="O5" s="32"/>
+      <c r="P5" s="31"/>
+      <c r="Q5" s="31"/>
+      <c r="R5" s="31"/>
+      <c r="S5" s="31"/>
       <c r="T5" s="9"/>
-      <c r="U5" s="23"/>
-      <c r="V5" s="23"/>
-      <c r="W5" s="23"/>
-      <c r="X5" s="23"/>
+      <c r="U5" s="31"/>
+      <c r="V5" s="31"/>
+      <c r="W5" s="31"/>
+      <c r="X5" s="31"/>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A6" s="10"/>
@@ -1377,19 +1380,19 @@
       <c r="G6" s="10"/>
       <c r="H6" s="10"/>
       <c r="L6" s="10"/>
-      <c r="N6" s="22" t="s">
+      <c r="N6" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="O6" s="22"/>
-      <c r="P6" s="23"/>
-      <c r="Q6" s="23"/>
-      <c r="R6" s="23"/>
-      <c r="S6" s="23"/>
+      <c r="O6" s="32"/>
+      <c r="P6" s="31"/>
+      <c r="Q6" s="31"/>
+      <c r="R6" s="31"/>
+      <c r="S6" s="31"/>
       <c r="T6" s="9"/>
-      <c r="U6" s="23"/>
-      <c r="V6" s="23"/>
-      <c r="W6" s="23"/>
-      <c r="X6" s="23"/>
+      <c r="U6" s="31"/>
+      <c r="V6" s="31"/>
+      <c r="W6" s="31"/>
+      <c r="X6" s="31"/>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
@@ -1406,19 +1409,19 @@
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
-      <c r="N7" s="22" t="s">
+      <c r="N7" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="O7" s="22"/>
-      <c r="P7" s="23"/>
-      <c r="Q7" s="23"/>
-      <c r="R7" s="23"/>
-      <c r="S7" s="23"/>
+      <c r="O7" s="32"/>
+      <c r="P7" s="31"/>
+      <c r="Q7" s="31"/>
+      <c r="R7" s="31"/>
+      <c r="S7" s="31"/>
       <c r="T7" s="9"/>
-      <c r="U7" s="23"/>
-      <c r="V7" s="23"/>
-      <c r="W7" s="23"/>
-      <c r="X7" s="23"/>
+      <c r="U7" s="31"/>
+      <c r="V7" s="31"/>
+      <c r="W7" s="31"/>
+      <c r="X7" s="31"/>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A8" s="5"/>
@@ -1433,19 +1436,19 @@
       <c r="J8" s="6"/>
       <c r="K8" s="6"/>
       <c r="L8" s="6"/>
-      <c r="N8" s="22" t="s">
+      <c r="N8" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="O8" s="22"/>
-      <c r="P8" s="23"/>
-      <c r="Q8" s="23"/>
-      <c r="R8" s="23"/>
-      <c r="S8" s="23"/>
+      <c r="O8" s="32"/>
+      <c r="P8" s="31"/>
+      <c r="Q8" s="31"/>
+      <c r="R8" s="31"/>
+      <c r="S8" s="31"/>
       <c r="T8" s="9"/>
-      <c r="U8" s="23"/>
-      <c r="V8" s="23"/>
-      <c r="W8" s="23"/>
-      <c r="X8" s="23"/>
+      <c r="U8" s="31"/>
+      <c r="V8" s="31"/>
+      <c r="W8" s="31"/>
+      <c r="X8" s="31"/>
     </row>
     <row r="9" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="10" t="s">
@@ -1461,19 +1464,19 @@
       <c r="J9" s="6"/>
       <c r="K9" s="6"/>
       <c r="L9" s="6"/>
-      <c r="N9" s="22" t="s">
+      <c r="N9" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="O9" s="22"/>
-      <c r="P9" s="23"/>
-      <c r="Q9" s="23"/>
-      <c r="R9" s="23"/>
-      <c r="S9" s="23"/>
+      <c r="O9" s="32"/>
+      <c r="P9" s="31"/>
+      <c r="Q9" s="31"/>
+      <c r="R9" s="31"/>
+      <c r="S9" s="31"/>
       <c r="T9" s="9"/>
-      <c r="U9" s="23"/>
-      <c r="V9" s="23"/>
-      <c r="W9" s="23"/>
-      <c r="X9" s="23"/>
+      <c r="U9" s="31"/>
+      <c r="V9" s="31"/>
+      <c r="W9" s="31"/>
+      <c r="X9" s="31"/>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A10" s="10"/>
@@ -1822,7 +1825,7 @@
       <c r="K24" s="19"/>
       <c r="L24" s="19"/>
       <c r="M24" s="4" t="s">
-        <v>1</v>
+        <v>43</v>
       </c>
       <c r="N24" s="3"/>
       <c r="O24" s="3"/>
@@ -2168,25 +2171,25 @@
       <c r="C39" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D39" s="29" t="s">
+      <c r="D39" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="30"/>
-      <c r="F39" s="29" t="s">
+      <c r="E39" s="24"/>
+      <c r="F39" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="G39" s="30"/>
+      <c r="G39" s="24"/>
       <c r="H39" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="I39" s="29" t="s">
+      <c r="I39" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="J39" s="30"/>
-      <c r="K39" s="29" t="s">
+      <c r="J39" s="24"/>
+      <c r="K39" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="L39" s="30"/>
+      <c r="L39" s="24"/>
       <c r="O39" s="6"/>
       <c r="P39" s="6"/>
       <c r="Q39" s="6"/>
@@ -2204,15 +2207,15 @@
       <c r="C40" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D40" s="31"/>
-      <c r="E40" s="32"/>
-      <c r="F40" s="31"/>
-      <c r="G40" s="32"/>
+      <c r="D40" s="21"/>
+      <c r="E40" s="22"/>
+      <c r="F40" s="21"/>
+      <c r="G40" s="22"/>
       <c r="H40" s="11"/>
-      <c r="I40" s="31"/>
-      <c r="J40" s="32"/>
-      <c r="K40" s="31"/>
-      <c r="L40" s="32"/>
+      <c r="I40" s="21"/>
+      <c r="J40" s="22"/>
+      <c r="K40" s="21"/>
+      <c r="L40" s="22"/>
       <c r="M40" s="10" t="s">
         <v>41</v>
       </c>
@@ -2231,15 +2234,15 @@
       <c r="C41" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D41" s="31"/>
-      <c r="E41" s="32"/>
-      <c r="F41" s="31"/>
-      <c r="G41" s="32"/>
+      <c r="D41" s="21"/>
+      <c r="E41" s="22"/>
+      <c r="F41" s="21"/>
+      <c r="G41" s="22"/>
       <c r="H41" s="11"/>
-      <c r="I41" s="31"/>
-      <c r="J41" s="32"/>
-      <c r="K41" s="31"/>
-      <c r="L41" s="32"/>
+      <c r="I41" s="21"/>
+      <c r="J41" s="22"/>
+      <c r="K41" s="21"/>
+      <c r="L41" s="22"/>
       <c r="O41" s="18"/>
       <c r="P41" s="19"/>
       <c r="Q41" s="19"/>
@@ -2255,15 +2258,15 @@
       <c r="C42" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="D42" s="31"/>
-      <c r="E42" s="32"/>
-      <c r="F42" s="31"/>
-      <c r="G42" s="32"/>
+      <c r="D42" s="21"/>
+      <c r="E42" s="22"/>
+      <c r="F42" s="21"/>
+      <c r="G42" s="22"/>
       <c r="H42" s="11"/>
-      <c r="I42" s="31"/>
-      <c r="J42" s="32"/>
-      <c r="K42" s="31"/>
-      <c r="L42" s="32"/>
+      <c r="I42" s="21"/>
+      <c r="J42" s="22"/>
+      <c r="K42" s="21"/>
+      <c r="L42" s="22"/>
       <c r="O42" s="6"/>
       <c r="P42" s="19"/>
       <c r="Q42" s="19"/>
@@ -2279,15 +2282,15 @@
       <c r="C43" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D43" s="31"/>
-      <c r="E43" s="32"/>
-      <c r="F43" s="31"/>
-      <c r="G43" s="32"/>
+      <c r="D43" s="21"/>
+      <c r="E43" s="22"/>
+      <c r="F43" s="21"/>
+      <c r="G43" s="22"/>
       <c r="H43" s="11"/>
-      <c r="I43" s="31"/>
-      <c r="J43" s="32"/>
-      <c r="K43" s="31"/>
-      <c r="L43" s="32"/>
+      <c r="I43" s="21"/>
+      <c r="J43" s="22"/>
+      <c r="K43" s="21"/>
+      <c r="L43" s="22"/>
       <c r="O43" s="6"/>
       <c r="P43" s="19"/>
       <c r="Q43" s="19"/>
@@ -2456,43 +2459,16 @@
     </row>
   </sheetData>
   <mergeCells count="56">
-    <mergeCell ref="I43:J43"/>
-    <mergeCell ref="I42:J42"/>
-    <mergeCell ref="I41:J41"/>
-    <mergeCell ref="I40:J40"/>
-    <mergeCell ref="I39:J39"/>
-    <mergeCell ref="K43:L43"/>
-    <mergeCell ref="K42:L42"/>
-    <mergeCell ref="K41:L41"/>
-    <mergeCell ref="K40:L40"/>
-    <mergeCell ref="K39:L39"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="F39:G39"/>
-    <mergeCell ref="F40:G40"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="P3:Q3"/>
-    <mergeCell ref="R3:S3"/>
-    <mergeCell ref="U3:V3"/>
-    <mergeCell ref="W3:X3"/>
-    <mergeCell ref="P4:Q4"/>
-    <mergeCell ref="R4:S4"/>
-    <mergeCell ref="U4:V4"/>
-    <mergeCell ref="W4:X4"/>
-    <mergeCell ref="P5:Q5"/>
-    <mergeCell ref="R5:S5"/>
-    <mergeCell ref="U5:V5"/>
-    <mergeCell ref="W5:X5"/>
-    <mergeCell ref="P6:Q6"/>
-    <mergeCell ref="R6:S6"/>
-    <mergeCell ref="U6:V6"/>
-    <mergeCell ref="W6:X6"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="N7:O7"/>
+    <mergeCell ref="N8:O8"/>
+    <mergeCell ref="N9:O9"/>
+    <mergeCell ref="P9:Q9"/>
+    <mergeCell ref="R9:S9"/>
+    <mergeCell ref="U9:V9"/>
     <mergeCell ref="W9:X9"/>
     <mergeCell ref="P7:Q7"/>
     <mergeCell ref="R7:S7"/>
@@ -2502,16 +2478,43 @@
     <mergeCell ref="R8:S8"/>
     <mergeCell ref="U8:V8"/>
     <mergeCell ref="W8:X8"/>
-    <mergeCell ref="N8:O8"/>
-    <mergeCell ref="N9:O9"/>
-    <mergeCell ref="P9:Q9"/>
-    <mergeCell ref="R9:S9"/>
-    <mergeCell ref="U9:V9"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="N4:O4"/>
-    <mergeCell ref="N5:O5"/>
-    <mergeCell ref="N6:O6"/>
-    <mergeCell ref="N7:O7"/>
+    <mergeCell ref="P5:Q5"/>
+    <mergeCell ref="R5:S5"/>
+    <mergeCell ref="U5:V5"/>
+    <mergeCell ref="W5:X5"/>
+    <mergeCell ref="P6:Q6"/>
+    <mergeCell ref="R6:S6"/>
+    <mergeCell ref="U6:V6"/>
+    <mergeCell ref="W6:X6"/>
+    <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="R3:S3"/>
+    <mergeCell ref="U3:V3"/>
+    <mergeCell ref="W3:X3"/>
+    <mergeCell ref="P4:Q4"/>
+    <mergeCell ref="R4:S4"/>
+    <mergeCell ref="U4:V4"/>
+    <mergeCell ref="W4:X4"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="F40:G40"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="K43:L43"/>
+    <mergeCell ref="K42:L42"/>
+    <mergeCell ref="K41:L41"/>
+    <mergeCell ref="K40:L40"/>
+    <mergeCell ref="K39:L39"/>
+    <mergeCell ref="I43:J43"/>
+    <mergeCell ref="I42:J42"/>
+    <mergeCell ref="I41:J41"/>
+    <mergeCell ref="I40:J40"/>
+    <mergeCell ref="I39:J39"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25297619047619047" top="0.25297619047619047" bottom="0.25297619047619047" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Modifications apportées suite ajouts RGPD
</commit_message>
<xml_diff>
--- a/public/dependencies/includes/Fiche info projet.xlsx
+++ b/public/dependencies/includes/Fiche info projet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\dev-requests\public\dependencies\includes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A8B182F-6307-4351-9ECC-A2279BB6472B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{266D4196-A149-47E1-8AFF-5044904EC240}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="150" windowWidth="24920" windowHeight="12080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
   <si>
     <t>DevReq</t>
   </si>
@@ -149,10 +149,16 @@
     <t>Processus lié</t>
   </si>
   <si>
-    <t>Impact</t>
-  </si>
-  <si>
     <t>Informations RGPD</t>
+  </si>
+  <si>
+    <t>Risque sur la vie privée</t>
+  </si>
+  <si>
+    <t>Commentaire DPO</t>
+  </si>
+  <si>
+    <t>Historique des statuts précédents</t>
   </si>
 </sst>
 </file>
@@ -719,20 +725,14 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -741,19 +741,25 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="78">
@@ -860,7 +866,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>4081</xdr:colOff>
+      <xdr:colOff>10431</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>12382</xdr:rowOff>
     </xdr:to>
@@ -1228,7 +1234,7 @@
   <dimension ref="A1:X54"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScale="55" zoomScaleNormal="70" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="55" workbookViewId="0">
-      <selection activeCell="M24" sqref="M24"/>
+      <selection activeCell="M49" sqref="M49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1250,7 +1256,7 @@
   <sheetData>
     <row r="1" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="28" t="s">
         <v>0</v>
       </c>
       <c r="M1" s="4" t="s">
@@ -1270,7 +1276,7 @@
     </row>
     <row r="2" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
-      <c r="B2" s="25"/>
+      <c r="B2" s="28"/>
       <c r="D2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1284,29 +1290,29 @@
       <c r="L2" s="6"/>
     </row>
     <row r="3" spans="1:24" ht="39" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="N3" s="28" t="s">
+      <c r="N3" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="O3" s="28"/>
-      <c r="P3" s="26" t="s">
+      <c r="O3" s="21"/>
+      <c r="P3" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="Q3" s="27"/>
-      <c r="R3" s="26" t="s">
+      <c r="Q3" s="25"/>
+      <c r="R3" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="S3" s="27"/>
+      <c r="S3" s="25"/>
       <c r="T3" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="U3" s="28" t="s">
+      <c r="U3" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="V3" s="28"/>
-      <c r="W3" s="29" t="s">
+      <c r="V3" s="21"/>
+      <c r="W3" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="X3" s="29"/>
+      <c r="X3" s="26"/>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A4" s="10" t="s">
@@ -1325,19 +1331,19 @@
       <c r="J4" s="6"/>
       <c r="K4" s="6"/>
       <c r="L4" s="6"/>
-      <c r="N4" s="32" t="s">
+      <c r="N4" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="O4" s="32"/>
-      <c r="P4" s="30"/>
-      <c r="Q4" s="30"/>
-      <c r="R4" s="31"/>
-      <c r="S4" s="31"/>
+      <c r="O4" s="22"/>
+      <c r="P4" s="27"/>
+      <c r="Q4" s="27"/>
+      <c r="R4" s="23"/>
+      <c r="S4" s="23"/>
       <c r="T4" s="9"/>
-      <c r="U4" s="31"/>
-      <c r="V4" s="31"/>
-      <c r="W4" s="31"/>
-      <c r="X4" s="31"/>
+      <c r="U4" s="23"/>
+      <c r="V4" s="23"/>
+      <c r="W4" s="23"/>
+      <c r="X4" s="23"/>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A5" s="10" t="s">
@@ -1356,19 +1362,19 @@
       <c r="J5" s="6"/>
       <c r="K5" s="6"/>
       <c r="L5" s="6"/>
-      <c r="N5" s="32" t="s">
+      <c r="N5" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="O5" s="32"/>
-      <c r="P5" s="31"/>
-      <c r="Q5" s="31"/>
-      <c r="R5" s="31"/>
-      <c r="S5" s="31"/>
+      <c r="O5" s="22"/>
+      <c r="P5" s="23"/>
+      <c r="Q5" s="23"/>
+      <c r="R5" s="23"/>
+      <c r="S5" s="23"/>
       <c r="T5" s="9"/>
-      <c r="U5" s="31"/>
-      <c r="V5" s="31"/>
-      <c r="W5" s="31"/>
-      <c r="X5" s="31"/>
+      <c r="U5" s="23"/>
+      <c r="V5" s="23"/>
+      <c r="W5" s="23"/>
+      <c r="X5" s="23"/>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A6" s="10"/>
@@ -1380,19 +1386,19 @@
       <c r="G6" s="10"/>
       <c r="H6" s="10"/>
       <c r="L6" s="10"/>
-      <c r="N6" s="32" t="s">
+      <c r="N6" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="O6" s="32"/>
-      <c r="P6" s="31"/>
-      <c r="Q6" s="31"/>
-      <c r="R6" s="31"/>
-      <c r="S6" s="31"/>
+      <c r="O6" s="22"/>
+      <c r="P6" s="23"/>
+      <c r="Q6" s="23"/>
+      <c r="R6" s="23"/>
+      <c r="S6" s="23"/>
       <c r="T6" s="9"/>
-      <c r="U6" s="31"/>
-      <c r="V6" s="31"/>
-      <c r="W6" s="31"/>
-      <c r="X6" s="31"/>
+      <c r="U6" s="23"/>
+      <c r="V6" s="23"/>
+      <c r="W6" s="23"/>
+      <c r="X6" s="23"/>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
@@ -1409,19 +1415,19 @@
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
-      <c r="N7" s="32" t="s">
+      <c r="N7" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="O7" s="32"/>
-      <c r="P7" s="31"/>
-      <c r="Q7" s="31"/>
-      <c r="R7" s="31"/>
-      <c r="S7" s="31"/>
+      <c r="O7" s="22"/>
+      <c r="P7" s="23"/>
+      <c r="Q7" s="23"/>
+      <c r="R7" s="23"/>
+      <c r="S7" s="23"/>
       <c r="T7" s="9"/>
-      <c r="U7" s="31"/>
-      <c r="V7" s="31"/>
-      <c r="W7" s="31"/>
-      <c r="X7" s="31"/>
+      <c r="U7" s="23"/>
+      <c r="V7" s="23"/>
+      <c r="W7" s="23"/>
+      <c r="X7" s="23"/>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A8" s="5"/>
@@ -1436,19 +1442,19 @@
       <c r="J8" s="6"/>
       <c r="K8" s="6"/>
       <c r="L8" s="6"/>
-      <c r="N8" s="32" t="s">
+      <c r="N8" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="O8" s="32"/>
-      <c r="P8" s="31"/>
-      <c r="Q8" s="31"/>
-      <c r="R8" s="31"/>
-      <c r="S8" s="31"/>
+      <c r="O8" s="22"/>
+      <c r="P8" s="23"/>
+      <c r="Q8" s="23"/>
+      <c r="R8" s="23"/>
+      <c r="S8" s="23"/>
       <c r="T8" s="9"/>
-      <c r="U8" s="31"/>
-      <c r="V8" s="31"/>
-      <c r="W8" s="31"/>
-      <c r="X8" s="31"/>
+      <c r="U8" s="23"/>
+      <c r="V8" s="23"/>
+      <c r="W8" s="23"/>
+      <c r="X8" s="23"/>
     </row>
     <row r="9" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="10" t="s">
@@ -1464,19 +1470,19 @@
       <c r="J9" s="6"/>
       <c r="K9" s="6"/>
       <c r="L9" s="6"/>
-      <c r="N9" s="32" t="s">
+      <c r="N9" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="O9" s="32"/>
-      <c r="P9" s="31"/>
-      <c r="Q9" s="31"/>
-      <c r="R9" s="31"/>
-      <c r="S9" s="31"/>
+      <c r="O9" s="22"/>
+      <c r="P9" s="23"/>
+      <c r="Q9" s="23"/>
+      <c r="R9" s="23"/>
+      <c r="S9" s="23"/>
       <c r="T9" s="9"/>
-      <c r="U9" s="31"/>
-      <c r="V9" s="31"/>
-      <c r="W9" s="31"/>
-      <c r="X9" s="31"/>
+      <c r="U9" s="23"/>
+      <c r="V9" s="23"/>
+      <c r="W9" s="23"/>
+      <c r="X9" s="23"/>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A10" s="10"/>
@@ -1720,18 +1726,20 @@
       <c r="X19" s="6"/>
     </row>
     <row r="20" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="M20" s="6"/>
-      <c r="N20" s="6"/>
-      <c r="O20" s="6"/>
-      <c r="P20" s="6"/>
-      <c r="Q20" s="6"/>
-      <c r="R20" s="6"/>
-      <c r="S20" s="6"/>
-      <c r="T20" s="6"/>
-      <c r="U20" s="6"/>
-      <c r="V20" s="6"/>
-      <c r="W20" s="6"/>
-      <c r="X20" s="6"/>
+      <c r="M20" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="N20" s="3"/>
+      <c r="O20" s="3"/>
+      <c r="P20" s="3"/>
+      <c r="Q20" s="3"/>
+      <c r="R20" s="3"/>
+      <c r="S20" s="3"/>
+      <c r="T20" s="3"/>
+      <c r="U20" s="3"/>
+      <c r="V20" s="3"/>
+      <c r="W20" s="3"/>
+      <c r="X20" s="3"/>
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A21" s="10"/>
@@ -1746,7 +1754,7 @@
       <c r="J21" s="6"/>
       <c r="K21" s="6"/>
       <c r="L21" s="6"/>
-      <c r="M21" s="6"/>
+      <c r="M21" s="5"/>
       <c r="N21" s="6"/>
       <c r="O21" s="6"/>
       <c r="P21" s="6"/>
@@ -1772,8 +1780,9 @@
       <c r="J22" s="6"/>
       <c r="K22" s="6"/>
       <c r="L22" s="6"/>
-      <c r="M22" s="5"/>
-      <c r="N22" s="6"/>
+      <c r="M22" s="10" t="s">
+        <v>39</v>
+      </c>
       <c r="O22" s="6"/>
       <c r="P22" s="6"/>
       <c r="Q22" s="6"/>
@@ -1798,8 +1807,6 @@
       <c r="J23" s="20"/>
       <c r="K23" s="20"/>
       <c r="L23" s="20"/>
-      <c r="M23" s="5"/>
-      <c r="N23" s="6"/>
       <c r="O23" s="6"/>
       <c r="P23" s="6"/>
       <c r="Q23" s="6"/>
@@ -1824,20 +1831,16 @@
       <c r="J24" s="19"/>
       <c r="K24" s="19"/>
       <c r="L24" s="19"/>
-      <c r="M24" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="N24" s="3"/>
-      <c r="O24" s="3"/>
-      <c r="P24" s="3"/>
-      <c r="Q24" s="3"/>
-      <c r="R24" s="3"/>
-      <c r="S24" s="3"/>
-      <c r="T24" s="3"/>
-      <c r="U24" s="3"/>
-      <c r="V24" s="3"/>
-      <c r="W24" s="3"/>
-      <c r="X24" s="3"/>
+      <c r="O24" s="6"/>
+      <c r="P24" s="6"/>
+      <c r="Q24" s="6"/>
+      <c r="R24" s="6"/>
+      <c r="S24" s="6"/>
+      <c r="T24" s="6"/>
+      <c r="U24" s="6"/>
+      <c r="V24" s="6"/>
+      <c r="W24" s="6"/>
+      <c r="X24" s="6"/>
     </row>
     <row r="25" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A25" s="10"/>
@@ -1852,8 +1855,6 @@
       <c r="J25" s="19"/>
       <c r="K25" s="19"/>
       <c r="L25" s="19"/>
-      <c r="M25" s="5"/>
-      <c r="N25" s="6"/>
       <c r="O25" s="6"/>
       <c r="P25" s="6"/>
       <c r="Q25" s="6"/>
@@ -1878,9 +1879,6 @@
       <c r="J26" s="19"/>
       <c r="K26" s="19"/>
       <c r="L26" s="19"/>
-      <c r="M26" s="10" t="s">
-        <v>39</v>
-      </c>
       <c r="O26" s="6"/>
       <c r="P26" s="6"/>
       <c r="Q26" s="6"/>
@@ -1907,6 +1905,9 @@
       <c r="J27" s="19"/>
       <c r="K27" s="19"/>
       <c r="L27" s="19"/>
+      <c r="M27" s="10" t="s">
+        <v>40</v>
+      </c>
       <c r="O27" s="6"/>
       <c r="P27" s="6"/>
       <c r="Q27" s="6"/>
@@ -2027,6 +2028,9 @@
       <c r="J32" s="6"/>
       <c r="K32" s="6"/>
       <c r="L32" s="6"/>
+      <c r="M32" s="10" t="s">
+        <v>41</v>
+      </c>
       <c r="O32" s="6"/>
       <c r="P32" s="6"/>
       <c r="Q32" s="6"/>
@@ -2051,19 +2055,6 @@
       <c r="J33" s="6"/>
       <c r="K33" s="6"/>
       <c r="L33" s="6"/>
-      <c r="M33" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="O33" s="6"/>
-      <c r="P33" s="6"/>
-      <c r="Q33" s="6"/>
-      <c r="R33" s="6"/>
-      <c r="S33" s="6"/>
-      <c r="T33" s="6"/>
-      <c r="U33" s="6"/>
-      <c r="V33" s="6"/>
-      <c r="W33" s="6"/>
-      <c r="X33" s="6"/>
     </row>
     <row r="34" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A34" s="10"/>
@@ -2117,18 +2108,18 @@
       <c r="G36" s="10"/>
       <c r="H36" s="10"/>
       <c r="L36" s="10"/>
-      <c r="O36" s="6"/>
-      <c r="P36" s="6"/>
-      <c r="Q36" s="6"/>
-      <c r="R36" s="6"/>
-      <c r="S36" s="6"/>
-      <c r="T36" s="6"/>
-      <c r="U36" s="6"/>
-      <c r="V36" s="6"/>
-      <c r="W36" s="6"/>
-      <c r="X36" s="6"/>
-    </row>
-    <row r="37" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="O36" s="16"/>
+      <c r="P36" s="20"/>
+      <c r="Q36" s="20"/>
+      <c r="R36" s="20"/>
+      <c r="S36" s="20"/>
+      <c r="T36" s="17"/>
+      <c r="U36" s="20"/>
+      <c r="V36" s="20"/>
+      <c r="W36" s="20"/>
+      <c r="X36" s="20"/>
+    </row>
+    <row r="37" spans="1:24" ht="16" x14ac:dyDescent="0.45">
       <c r="A37" s="4" t="s">
         <v>21</v>
       </c>
@@ -2143,6 +2134,19 @@
       <c r="J37" s="3"/>
       <c r="K37" s="3"/>
       <c r="L37" s="3"/>
+      <c r="M37" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="O37" s="18"/>
+      <c r="P37" s="19"/>
+      <c r="Q37" s="19"/>
+      <c r="R37" s="19"/>
+      <c r="S37" s="19"/>
+      <c r="T37" s="15"/>
+      <c r="U37" s="19"/>
+      <c r="V37" s="19"/>
+      <c r="W37" s="19"/>
+      <c r="X37" s="19"/>
     </row>
     <row r="38" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A38" s="5"/>
@@ -2155,15 +2159,15 @@
       <c r="H38" s="10"/>
       <c r="L38" s="10"/>
       <c r="O38" s="6"/>
-      <c r="P38" s="6"/>
-      <c r="Q38" s="6"/>
-      <c r="R38" s="6"/>
-      <c r="S38" s="6"/>
-      <c r="T38" s="6"/>
-      <c r="U38" s="6"/>
-      <c r="V38" s="6"/>
-      <c r="W38" s="6"/>
-      <c r="X38" s="6"/>
+      <c r="P38" s="19"/>
+      <c r="Q38" s="19"/>
+      <c r="R38" s="19"/>
+      <c r="S38" s="19"/>
+      <c r="T38" s="15"/>
+      <c r="U38" s="19"/>
+      <c r="V38" s="19"/>
+      <c r="W38" s="19"/>
+      <c r="X38" s="19"/>
     </row>
     <row r="39" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A39" s="10"/>
@@ -2171,35 +2175,35 @@
       <c r="C39" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D39" s="23" t="s">
+      <c r="D39" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="24"/>
-      <c r="F39" s="23" t="s">
+      <c r="E39" s="30"/>
+      <c r="F39" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="G39" s="24"/>
+      <c r="G39" s="30"/>
       <c r="H39" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="I39" s="23" t="s">
+      <c r="I39" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="J39" s="24"/>
-      <c r="K39" s="23" t="s">
+      <c r="J39" s="30"/>
+      <c r="K39" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="L39" s="24"/>
+      <c r="L39" s="30"/>
       <c r="O39" s="6"/>
-      <c r="P39" s="6"/>
-      <c r="Q39" s="6"/>
-      <c r="R39" s="6"/>
-      <c r="S39" s="6"/>
-      <c r="T39" s="6"/>
-      <c r="U39" s="6"/>
-      <c r="V39" s="6"/>
-      <c r="W39" s="6"/>
-      <c r="X39" s="6"/>
+      <c r="P39" s="19"/>
+      <c r="Q39" s="19"/>
+      <c r="R39" s="19"/>
+      <c r="S39" s="19"/>
+      <c r="T39" s="15"/>
+      <c r="U39" s="19"/>
+      <c r="V39" s="19"/>
+      <c r="W39" s="19"/>
+      <c r="X39" s="19"/>
     </row>
     <row r="40" spans="1:24" ht="16" x14ac:dyDescent="0.45">
       <c r="A40" s="10"/>
@@ -2207,113 +2211,72 @@
       <c r="C40" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D40" s="21"/>
-      <c r="E40" s="22"/>
-      <c r="F40" s="21"/>
-      <c r="G40" s="22"/>
+      <c r="D40" s="31"/>
+      <c r="E40" s="32"/>
+      <c r="F40" s="31"/>
+      <c r="G40" s="32"/>
       <c r="H40" s="11"/>
-      <c r="I40" s="21"/>
-      <c r="J40" s="22"/>
-      <c r="K40" s="21"/>
-      <c r="L40" s="22"/>
-      <c r="M40" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="O40" s="16"/>
-      <c r="P40" s="20"/>
-      <c r="Q40" s="20"/>
-      <c r="R40" s="20"/>
-      <c r="S40" s="20"/>
-      <c r="T40" s="17"/>
-      <c r="U40" s="20"/>
-      <c r="V40" s="20"/>
-      <c r="W40" s="20"/>
-      <c r="X40" s="20"/>
-    </row>
-    <row r="41" spans="1:24" s="10" customFormat="1" ht="16" x14ac:dyDescent="0.45">
+      <c r="I40" s="31"/>
+      <c r="J40" s="32"/>
+      <c r="K40" s="31"/>
+      <c r="L40" s="32"/>
+      <c r="O40" s="6"/>
+      <c r="P40" s="19"/>
+      <c r="Q40" s="19"/>
+      <c r="R40" s="19"/>
+      <c r="S40" s="19"/>
+      <c r="T40" s="15"/>
+      <c r="U40" s="19"/>
+      <c r="V40" s="19"/>
+      <c r="W40" s="19"/>
+      <c r="X40" s="19"/>
+    </row>
+    <row r="41" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="C41" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D41" s="21"/>
-      <c r="E41" s="22"/>
-      <c r="F41" s="21"/>
-      <c r="G41" s="22"/>
+      <c r="D41" s="31"/>
+      <c r="E41" s="32"/>
+      <c r="F41" s="31"/>
+      <c r="G41" s="32"/>
       <c r="H41" s="11"/>
-      <c r="I41" s="21"/>
-      <c r="J41" s="22"/>
-      <c r="K41" s="21"/>
-      <c r="L41" s="22"/>
-      <c r="O41" s="18"/>
-      <c r="P41" s="19"/>
-      <c r="Q41" s="19"/>
-      <c r="R41" s="19"/>
-      <c r="S41" s="19"/>
-      <c r="T41" s="15"/>
-      <c r="U41" s="19"/>
-      <c r="V41" s="19"/>
-      <c r="W41" s="19"/>
-      <c r="X41" s="19"/>
+      <c r="I41" s="31"/>
+      <c r="J41" s="32"/>
+      <c r="K41" s="31"/>
+      <c r="L41" s="32"/>
     </row>
     <row r="42" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="C42" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="D42" s="21"/>
-      <c r="E42" s="22"/>
-      <c r="F42" s="21"/>
-      <c r="G42" s="22"/>
+      <c r="D42" s="31"/>
+      <c r="E42" s="32"/>
+      <c r="F42" s="31"/>
+      <c r="G42" s="32"/>
       <c r="H42" s="11"/>
-      <c r="I42" s="21"/>
-      <c r="J42" s="22"/>
-      <c r="K42" s="21"/>
-      <c r="L42" s="22"/>
-      <c r="O42" s="6"/>
-      <c r="P42" s="19"/>
-      <c r="Q42" s="19"/>
-      <c r="R42" s="19"/>
-      <c r="S42" s="19"/>
-      <c r="T42" s="15"/>
-      <c r="U42" s="19"/>
-      <c r="V42" s="19"/>
-      <c r="W42" s="19"/>
-      <c r="X42" s="19"/>
+      <c r="I42" s="31"/>
+      <c r="J42" s="32"/>
+      <c r="K42" s="31"/>
+      <c r="L42" s="32"/>
+      <c r="M42" s="10" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="43" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="C43" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D43" s="21"/>
-      <c r="E43" s="22"/>
-      <c r="F43" s="21"/>
-      <c r="G43" s="22"/>
+      <c r="D43" s="31"/>
+      <c r="E43" s="32"/>
+      <c r="F43" s="31"/>
+      <c r="G43" s="32"/>
       <c r="H43" s="11"/>
-      <c r="I43" s="21"/>
-      <c r="J43" s="22"/>
-      <c r="K43" s="21"/>
-      <c r="L43" s="22"/>
-      <c r="O43" s="6"/>
-      <c r="P43" s="19"/>
-      <c r="Q43" s="19"/>
-      <c r="R43" s="19"/>
-      <c r="S43" s="19"/>
-      <c r="T43" s="15"/>
-      <c r="U43" s="19"/>
-      <c r="V43" s="19"/>
-      <c r="W43" s="19"/>
-      <c r="X43" s="19"/>
-    </row>
-    <row r="44" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="O44" s="6"/>
-      <c r="P44" s="19"/>
-      <c r="Q44" s="19"/>
-      <c r="R44" s="19"/>
-      <c r="S44" s="19"/>
-      <c r="T44" s="15"/>
-      <c r="U44" s="19"/>
-      <c r="V44" s="19"/>
-      <c r="W44" s="19"/>
-      <c r="X44" s="19"/>
-    </row>
+      <c r="I43" s="31"/>
+      <c r="J43" s="32"/>
+      <c r="K43" s="31"/>
+      <c r="L43" s="32"/>
+    </row>
+    <row r="44" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
     <row r="45" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A45" s="4" t="s">
         <v>20</v>
@@ -2358,11 +2321,23 @@
       <c r="J47" s="6"/>
       <c r="K47" s="6"/>
       <c r="L47" s="10"/>
-      <c r="M47" s="10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="48" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    </row>
+    <row r="48" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="M48" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="N48" s="3"/>
+      <c r="O48" s="3"/>
+      <c r="P48" s="3"/>
+      <c r="Q48" s="3"/>
+      <c r="R48" s="3"/>
+      <c r="S48" s="3"/>
+      <c r="T48" s="3"/>
+      <c r="U48" s="3"/>
+      <c r="V48" s="3"/>
+      <c r="W48" s="3"/>
+      <c r="X48" s="3"/>
+    </row>
     <row r="49" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A49" s="4" t="s">
         <v>22</v>
@@ -2459,16 +2434,43 @@
     </row>
   </sheetData>
   <mergeCells count="56">
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="N4:O4"/>
-    <mergeCell ref="N5:O5"/>
-    <mergeCell ref="N6:O6"/>
-    <mergeCell ref="N7:O7"/>
-    <mergeCell ref="N8:O8"/>
-    <mergeCell ref="N9:O9"/>
-    <mergeCell ref="P9:Q9"/>
-    <mergeCell ref="R9:S9"/>
-    <mergeCell ref="U9:V9"/>
+    <mergeCell ref="I43:J43"/>
+    <mergeCell ref="I42:J42"/>
+    <mergeCell ref="I41:J41"/>
+    <mergeCell ref="I40:J40"/>
+    <mergeCell ref="I39:J39"/>
+    <mergeCell ref="K43:L43"/>
+    <mergeCell ref="K42:L42"/>
+    <mergeCell ref="K41:L41"/>
+    <mergeCell ref="K40:L40"/>
+    <mergeCell ref="K39:L39"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="F40:G40"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="R3:S3"/>
+    <mergeCell ref="U3:V3"/>
+    <mergeCell ref="W3:X3"/>
+    <mergeCell ref="P4:Q4"/>
+    <mergeCell ref="R4:S4"/>
+    <mergeCell ref="U4:V4"/>
+    <mergeCell ref="W4:X4"/>
+    <mergeCell ref="P5:Q5"/>
+    <mergeCell ref="R5:S5"/>
+    <mergeCell ref="U5:V5"/>
+    <mergeCell ref="W5:X5"/>
+    <mergeCell ref="P6:Q6"/>
+    <mergeCell ref="R6:S6"/>
+    <mergeCell ref="U6:V6"/>
+    <mergeCell ref="W6:X6"/>
     <mergeCell ref="W9:X9"/>
     <mergeCell ref="P7:Q7"/>
     <mergeCell ref="R7:S7"/>
@@ -2478,43 +2480,16 @@
     <mergeCell ref="R8:S8"/>
     <mergeCell ref="U8:V8"/>
     <mergeCell ref="W8:X8"/>
-    <mergeCell ref="P5:Q5"/>
-    <mergeCell ref="R5:S5"/>
-    <mergeCell ref="U5:V5"/>
-    <mergeCell ref="W5:X5"/>
-    <mergeCell ref="P6:Q6"/>
-    <mergeCell ref="R6:S6"/>
-    <mergeCell ref="U6:V6"/>
-    <mergeCell ref="W6:X6"/>
-    <mergeCell ref="P3:Q3"/>
-    <mergeCell ref="R3:S3"/>
-    <mergeCell ref="U3:V3"/>
-    <mergeCell ref="W3:X3"/>
-    <mergeCell ref="P4:Q4"/>
-    <mergeCell ref="R4:S4"/>
-    <mergeCell ref="U4:V4"/>
-    <mergeCell ref="W4:X4"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="F39:G39"/>
-    <mergeCell ref="F40:G40"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="K43:L43"/>
-    <mergeCell ref="K42:L42"/>
-    <mergeCell ref="K41:L41"/>
-    <mergeCell ref="K40:L40"/>
-    <mergeCell ref="K39:L39"/>
-    <mergeCell ref="I43:J43"/>
-    <mergeCell ref="I42:J42"/>
-    <mergeCell ref="I41:J41"/>
-    <mergeCell ref="I40:J40"/>
-    <mergeCell ref="I39:J39"/>
+    <mergeCell ref="N8:O8"/>
+    <mergeCell ref="N9:O9"/>
+    <mergeCell ref="P9:Q9"/>
+    <mergeCell ref="R9:S9"/>
+    <mergeCell ref="U9:V9"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="N7:O7"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25297619047619047" top="0.25297619047619047" bottom="0.25297619047619047" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>